<commit_message>
Final changes do data analysis and graphics
</commit_message>
<xml_diff>
--- a/Data Results_test_08.xlsx
+++ b/Data Results_test_08.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renato\CLionProjects\cp2020-2021_g26_45616_52360_52393\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764DED7F-C4BA-4AD5-A605-EC5C23263D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1ADC77F-6F06-41E5-BE95-25949C7594E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{FE04AF36-4D43-4F52-8DE8-9BA373B3A9EA}"/>
   </bookViews>
@@ -84,18 +84,87 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -105,127 +174,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -347,6 +295,62 @@
       </right>
       <top/>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -357,67 +361,67 @@
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -737,7 +741,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -747,295 +751,295 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="12">
         <v>2.4640719999999998</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="13">
         <v>1.4236120000000001</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
+      <c r="A4" s="6">
         <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>2.470189</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="9">
         <v>1.443182</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
+      <c r="A5" s="6">
         <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>2.471886</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="9">
         <v>1.456202</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
+      <c r="A6" s="6">
         <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>2.473112</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="9">
         <v>1.4576389999999999</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
+      <c r="A7" s="6">
         <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>2.4743179999999998</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="9">
         <v>1.458987</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
+      <c r="A8" s="6">
         <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>2.4745029999999999</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="9">
         <v>1.4602390000000001</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
+      <c r="A9" s="6">
         <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>2.4745940000000002</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="9">
         <v>1.4603569999999999</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
+      <c r="A10" s="6">
         <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>2.4747490000000001</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="9">
         <v>1.467452</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
+      <c r="A11" s="6">
         <v>9</v>
       </c>
       <c r="B11" s="1">
         <v>2.4748380000000001</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="9">
         <v>1.4683619999999999</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
+      <c r="A12" s="6">
         <v>10</v>
       </c>
       <c r="B12" s="1">
         <v>2.475025</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="9">
         <v>1.469422</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="8">
+      <c r="A13" s="6">
         <v>11</v>
       </c>
       <c r="B13" s="1">
         <v>2.4752540000000001</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="9">
         <v>1.4720329999999999</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="8">
+      <c r="A14" s="6">
         <v>12</v>
       </c>
       <c r="B14" s="1">
         <v>2.4756089999999999</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="9">
         <v>1.474197</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="8">
+      <c r="A15" s="6">
         <v>13</v>
       </c>
       <c r="B15" s="1">
         <v>2.4758019999999998</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="9">
         <v>1.4754400000000001</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="8">
+      <c r="A16" s="6">
         <v>14</v>
       </c>
       <c r="B16" s="1">
         <v>2.476585</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="9">
         <v>1.4759770000000001</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="8">
+      <c r="A17" s="6">
         <v>15</v>
       </c>
       <c r="B17" s="1">
         <v>2.4783379999999999</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="9">
         <v>1.4835480000000001</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="8">
+      <c r="A18" s="6">
         <v>16</v>
       </c>
       <c r="B18" s="1">
         <v>2.479123</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="9">
         <v>1.484245</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="8">
+      <c r="A19" s="6">
         <v>17</v>
       </c>
       <c r="B19" s="1">
         <v>2.4804919999999999</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="9">
         <v>1.487511</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="8">
+      <c r="A20" s="6">
         <v>18</v>
       </c>
       <c r="B20" s="1">
         <v>2.4822320000000002</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="9">
         <v>1.4896750000000001</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="8">
+      <c r="A21" s="6">
         <v>19</v>
       </c>
       <c r="B21" s="1">
         <v>2.4823680000000001</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="9">
         <v>1.4977240000000001</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="8">
+      <c r="A22" s="6">
         <v>20</v>
       </c>
       <c r="B22" s="1">
         <v>2.4828480000000002</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="9">
         <v>1.499287</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="8">
+      <c r="A23" s="6">
         <v>21</v>
       </c>
       <c r="B23" s="1">
         <v>2.4831300000000001</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="9">
         <v>1.501779</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="8">
+      <c r="A24" s="6">
         <v>22</v>
       </c>
       <c r="B24" s="1">
         <v>2.484947</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="9">
         <v>1.504904</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="8">
+      <c r="A25" s="6">
         <v>23</v>
       </c>
       <c r="B25" s="1">
         <v>2.4887619999999999</v>
       </c>
-      <c r="C25" s="13">
+      <c r="C25" s="9">
         <v>1.5162800000000001</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="8">
+      <c r="A26" s="6">
         <v>24</v>
       </c>
       <c r="B26" s="1">
         <v>2.4917310000000001</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="9">
         <v>1.5231760000000001</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="9">
+      <c r="A27" s="7">
         <v>25</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>2.4929890000000001</v>
       </c>
-      <c r="C27" s="14">
+      <c r="C27" s="10">
         <v>1.5326960000000001</v>
       </c>
     </row>
@@ -1043,11 +1047,11 @@
       <c r="A28" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="18">
         <f>AVERAGE(B3:B27)</f>
         <v>2.47829984</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="11">
         <f>AVERAGE(C3:C27)</f>
         <v>1.4793570400000005</v>
       </c>
@@ -1056,7 +1060,7 @@
       <c r="A29" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="16">
+      <c r="B29" s="19">
         <f>B28/C28</f>
         <v>1.6752547038948753</v>
       </c>

</xml_diff>